<commit_message>
product page not finish
</commit_message>
<xml_diff>
--- a/week6/作業進度.xlsx
+++ b/week6/作業進度.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="14805" windowHeight="7965"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>新增產品列表</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>添加footer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>設計產品畫面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加cart button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>設計個別產品畫面</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -74,18 +86,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -106,7 +112,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,13 +120,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:C10"/>
+  <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -439,46 +439,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -486,22 +486,36 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>